<commit_message>
LinReg, P@k, minor improvements
- Finalized LinReg
- Improved P@k
- Cleaned notebooks
- Improved folder structure
</commit_message>
<xml_diff>
--- a/data/categories_info.xlsx
+++ b/data/categories_info.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kvnstz/Documents/GitHub/MAT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872395D1-C849-2740-846F-741128C57D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA779816-5FC6-A444-814B-559813AD37D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="24460" windowWidth="28800" windowHeight="17540" xr2:uid="{00CD8DFE-16D9-DE42-A823-5D76E07612EF}"/>
+    <workbookView xWindow="7020" yWindow="3500" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00CD8DFE-16D9-DE42-A823-5D76E07612EF}"/>
   </bookViews>
   <sheets>
     <sheet name="CatXSurvey" sheetId="8" r:id="rId1"/>
     <sheet name="SparqlLookup" sheetId="6" r:id="rId2"/>
+    <sheet name="LinearRegr" sheetId="10" r:id="rId3"/>
+    <sheet name="CorrCoef" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>Category</t>
   </si>
@@ -189,6 +191,102 @@
   </si>
   <si>
     <t>Survey+</t>
+  </si>
+  <si>
+    <t>Eigenvector</t>
+  </si>
+  <si>
+    <t>PageRank</t>
+  </si>
+  <si>
+    <t>Eigenvector / PageRank</t>
+  </si>
+  <si>
+    <t>coefficient</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>GCM</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>0,001***</t>
+  </si>
+  <si>
+    <t>0,008**</t>
+  </si>
+  <si>
+    <t>0,005**</t>
+  </si>
+  <si>
+    <t>0,002**</t>
+  </si>
+  <si>
+    <t>0,031*</t>
+  </si>
+  <si>
+    <t>0,05*</t>
+  </si>
+  <si>
+    <t>0,014*</t>
+  </si>
+  <si>
+    <t>0,02*</t>
+  </si>
+  <si>
+    <t>0,011*</t>
+  </si>
+  <si>
+    <t>0,022*</t>
+  </si>
+  <si>
+    <t>0,006**</t>
+  </si>
+  <si>
+    <t>p &lt; 0,01</t>
+  </si>
+  <si>
+    <t>p &lt; 0,05</t>
+  </si>
+  <si>
+    <t>p &lt; 0,001</t>
+  </si>
+  <si>
+    <t>Significance of</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Correlation coefficient</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>Spearman</t>
+  </si>
+  <si>
+    <t>eigenvector-degree</t>
+  </si>
+  <si>
+    <t>pagerank-degree</t>
+  </si>
+  <si>
+    <t>pagerank-eigenvector</t>
+  </si>
+  <si>
+    <t>Prio class</t>
   </si>
 </sst>
 </file>
@@ -220,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +349,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -280,20 +402,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -608,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6968C97-1CC6-4C43-99B2-F2AD861BC1FB}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,9 +864,10 @@
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,21 +880,24 @@
       <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="I1" s="31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B2">
@@ -665,7 +909,7 @@
       <c r="D2">
         <v>98</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="37">
         <v>0.80989999999999995</v>
       </c>
       <c r="F2">
@@ -674,12 +918,15 @@
       <c r="G2">
         <v>56</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="33">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="I2" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -691,7 +938,7 @@
       <c r="D3">
         <v>80</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="33">
         <f>D3/C3</f>
         <v>0.55944055944055948</v>
       </c>
@@ -701,12 +948,15 @@
       <c r="G3">
         <v>69</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="33">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B4">
@@ -718,7 +968,7 @@
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="33">
         <f>D4/C4</f>
         <v>0.21428571428571427</v>
       </c>
@@ -728,12 +978,15 @@
       <c r="G4">
         <v>5</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="33">
         <v>0.13157894736842105</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B5">
@@ -745,7 +998,7 @@
       <c r="D5">
         <v>172</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="33">
         <f t="shared" ref="E5:E24" si="0">D5/C5</f>
         <v>0.94505494505494503</v>
       </c>
@@ -755,12 +1008,15 @@
       <c r="G5">
         <v>139</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="33">
         <v>0.89102564102564108</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="I5" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B6">
@@ -772,7 +1028,7 @@
       <c r="D6">
         <v>125</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="33">
         <f t="shared" si="0"/>
         <v>0.87412587412587417</v>
       </c>
@@ -782,12 +1038,15 @@
       <c r="G6">
         <v>119</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="33">
         <v>0.8623188405797102</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="I6" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B7">
@@ -799,7 +1058,7 @@
       <c r="D7">
         <v>72</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="33">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
@@ -809,12 +1068,15 @@
       <c r="G7">
         <v>73</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="33">
         <v>0.96052631578947367</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="I7" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B8">
@@ -826,7 +1088,7 @@
       <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="33">
         <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
@@ -836,12 +1098,15 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B9">
@@ -853,7 +1118,7 @@
       <c r="D9">
         <v>85</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="33">
         <f t="shared" si="0"/>
         <v>0.9550561797752809</v>
       </c>
@@ -863,12 +1128,15 @@
       <c r="G9">
         <v>82</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="33">
         <v>0.91111111111111109</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="I9" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -880,7 +1148,7 @@
       <c r="D10">
         <v>42</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="33">
         <f t="shared" si="0"/>
         <v>0.52500000000000002</v>
       </c>
@@ -890,12 +1158,15 @@
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="33">
         <v>0.2857142857142857</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="I10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B11">
@@ -907,7 +1178,7 @@
       <c r="D11">
         <v>28</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="33">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -917,12 +1188,15 @@
       <c r="G11">
         <v>17</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="33">
         <v>0.32692307692307693</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B12">
@@ -934,7 +1208,7 @@
       <c r="D12">
         <v>7</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="33">
         <f t="shared" si="0"/>
         <v>0.2413793103448276</v>
       </c>
@@ -944,12 +1218,15 @@
       <c r="G12">
         <v>4</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="33">
         <v>0.14285714285714285</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B13">
@@ -961,7 +1238,7 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="33">
         <f t="shared" si="0"/>
         <v>3.4482758620689655E-2</v>
       </c>
@@ -971,12 +1248,15 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B14">
@@ -988,7 +1268,7 @@
       <c r="D14">
         <v>7</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="33">
         <f t="shared" si="0"/>
         <v>0.21212121212121213</v>
       </c>
@@ -998,12 +1278,15 @@
       <c r="G14">
         <v>7</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="33">
         <v>0.21212121212121213</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B15">
@@ -1015,7 +1298,7 @@
       <c r="D15">
         <v>7</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="33">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
@@ -1025,12 +1308,15 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="33">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B16">
@@ -1042,7 +1328,7 @@
       <c r="D16">
         <v>52</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="33">
         <f t="shared" si="0"/>
         <v>0.85245901639344257</v>
       </c>
@@ -1052,12 +1338,15 @@
       <c r="G16">
         <v>27</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="33">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="I16" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B17">
@@ -1069,7 +1358,7 @@
       <c r="D17">
         <v>22</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="33">
         <f t="shared" si="0"/>
         <v>0.75862068965517238</v>
       </c>
@@ -1079,12 +1368,15 @@
       <c r="G17">
         <v>11</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="33">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="I17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B18">
@@ -1096,7 +1388,7 @@
       <c r="D18">
         <v>27</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="33">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
@@ -1106,12 +1398,15 @@
       <c r="G18">
         <v>16</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="33">
         <v>0.59259259259259256</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="I18" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B19">
@@ -1123,7 +1418,7 @@
       <c r="D19">
         <v>17</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="33">
         <f t="shared" si="0"/>
         <v>0.40476190476190477</v>
       </c>
@@ -1133,12 +1428,15 @@
       <c r="G19">
         <v>8</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="33">
         <v>0.21621621621621623</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B20">
@@ -1150,7 +1448,7 @@
       <c r="D20">
         <v>17</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="33">
         <f t="shared" si="0"/>
         <v>0.54838709677419351</v>
       </c>
@@ -1160,12 +1458,15 @@
       <c r="G20">
         <v>9</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="33">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B21">
@@ -1177,7 +1478,7 @@
       <c r="D21">
         <v>59</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="33">
         <f t="shared" si="0"/>
         <v>0.90769230769230769</v>
       </c>
@@ -1187,12 +1488,15 @@
       <c r="G21">
         <v>55</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="33">
         <v>0.859375</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="I21" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B22">
@@ -1204,7 +1508,7 @@
       <c r="D22">
         <v>47</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="33">
         <f t="shared" si="0"/>
         <v>0.78333333333333333</v>
       </c>
@@ -1214,12 +1518,15 @@
       <c r="G22">
         <v>37</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="33">
         <v>0.69811320754716977</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="I22" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B23">
@@ -1231,7 +1538,7 @@
       <c r="D23">
         <v>83</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1241,52 +1548,70 @@
       <c r="G23">
         <v>76</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="I23" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>289681</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>36</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>35</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="34">
         <f t="shared" si="0"/>
         <v>0.97222222222222221</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>34</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>31</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="34">
         <v>0.91176470588235292</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
+      <c r="I24" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="37">
         <f>SUM(E2:E24)/COUNTA(E2:E24)</f>
         <v>0.65664206821939675</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="37">
         <f>SUM(H2:H24)/COUNTA(H2:H24)</f>
         <v>0.49741615778529313</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H25">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1298,7 +1623,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1319,7 +1644,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1334,7 +1659,7 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="26" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1345,6 +1670,7 @@
       <c r="B2" s="3">
         <v>14010</v>
       </c>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1353,7 +1679,7 @@
       <c r="B3" s="3">
         <v>20069</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>4842</v>
       </c>
     </row>
@@ -1364,7 +1690,7 @@
       <c r="B4" s="3">
         <v>12389</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>63</v>
       </c>
     </row>
@@ -1375,6 +1701,7 @@
       <c r="B5" s="3">
         <v>73521</v>
       </c>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1383,7 +1710,7 @@
       <c r="B6">
         <v>4967</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="35">
         <v>5110</v>
       </c>
     </row>
@@ -1394,6 +1721,7 @@
       <c r="B7" s="3">
         <v>186953</v>
       </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1402,6 +1730,7 @@
       <c r="B8" s="3">
         <v>48</v>
       </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1410,6 +1739,7 @@
       <c r="B9" s="3">
         <v>35201</v>
       </c>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1418,7 +1748,7 @@
       <c r="B10" s="3">
         <v>11809</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>31</v>
       </c>
     </row>
@@ -1429,7 +1759,7 @@
       <c r="B11" s="3">
         <v>31528</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>36</v>
       </c>
     </row>
@@ -1440,6 +1770,7 @@
       <c r="B12" s="3">
         <v>53</v>
       </c>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1448,6 +1779,7 @@
       <c r="B13" s="3">
         <v>54</v>
       </c>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1456,7 +1788,7 @@
       <c r="B14">
         <v>58</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="35">
         <v>67</v>
       </c>
     </row>
@@ -1467,7 +1799,7 @@
       <c r="B15">
         <v>20</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="35">
         <v>22</v>
       </c>
     </row>
@@ -1478,6 +1810,7 @@
       <c r="B16" s="3">
         <v>63943</v>
       </c>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1486,6 +1819,7 @@
       <c r="B17" s="3">
         <v>17563</v>
       </c>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1494,6 +1828,7 @@
       <c r="B18" s="3">
         <v>11780</v>
       </c>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1502,6 +1837,7 @@
       <c r="B19" s="3">
         <v>4398</v>
       </c>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1510,7 +1846,7 @@
       <c r="B20">
         <v>968</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="35">
         <v>6114</v>
       </c>
     </row>
@@ -1521,7 +1857,7 @@
       <c r="B21">
         <v>505</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="35">
         <v>1470</v>
       </c>
     </row>
@@ -1532,6 +1868,7 @@
       <c r="B22" s="3">
         <v>28</v>
       </c>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1540,16 +1877,559 @@
       <c r="B23" s="3">
         <v>1178</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>685</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="36">
         <v>289681</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFDEED4-DD79-CC4B-BB52-AC8A8B12DBA7}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="K2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>1.7565999999999999</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.9859</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="H4">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>-6.4000000000000003E-3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="H5">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="D6">
+        <v>-1E-4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F6">
+        <v>-8.9999999999999998E-4</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="D7">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="F7">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="H7">
+        <v>-1E-4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F8">
+        <v>-3.2300000000000002E-2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.95E-2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <v>1.78E-2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.106</v>
+      </c>
+      <c r="H10">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>-3.0099999999999998E-2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D11">
+        <v>-1.9300000000000001E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="F11">
+        <v>-2.9899999999999999E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.155</v>
+      </c>
+      <c r="H11">
+        <v>-3.8600000000000002E-2</v>
+      </c>
+      <c r="I11" s="8">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>3.1349999999999998</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1.5665</v>
+      </c>
+      <c r="G12" s="8">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H12">
+        <v>4.9500000000000002E-2</v>
+      </c>
+      <c r="I12" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.107</v>
+      </c>
+      <c r="D13">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="F13">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="H13">
+        <v>1.9E-3</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>17.140499999999999</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>6.2286999999999999</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="H14">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.315</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-12.262</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-12.090999999999999</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF719BA7-282E-144E-8834-1DB729603BA3}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>0.60861409</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.277860621295827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3">
+        <v>0.95806588000000004</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.91790171333267501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.52535622000000004</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.203893461750626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>